<commit_message>
Minor updates to final paper
Minor updates to final paper (editing my section, highlighting things I know we need fixed [that we discussed]).  More rigurous (but I think still wrong) stress values from the MATLAB code
</commit_message>
<xml_diff>
--- a/finalPapers/MatlabResults.xlsx
+++ b/finalPapers/MatlabResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\420GroupProj\AE420-ME471-CSE451-GroupProject\finalPapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11D1D64-B5C0-48BC-A841-A791775A432F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BC42BA-243A-4DEC-8D40-03D4CA39674B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11925" xr2:uid="{228C8538-B6D7-47A5-9262-4F835E70FB31}"/>
   </bookViews>
@@ -1434,7 +1434,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,11 +1527,11 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>130.1</v>
+        <v>72</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C4:C7" si="0">100*ABS(B6-B7)/(B6)</f>
-        <v>67.97144263909405</v>
+        <f t="shared" ref="C7" si="0">100*ABS(B6-B7)/(B6)</f>
+        <v>82.274741506646976</v>
       </c>
       <c r="E7">
         <v>60</v>

</xml_diff>